<commit_message>
refactoring, an attempt at gen excel as well, updated countries
</commit_message>
<xml_diff>
--- a/process_irnw_inst-cap_intermediate.xlsx
+++ b/process_irnw_inst-cap_intermediate.xlsx
@@ -7,35 +7,35 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="AT" sheetId="1" r:id="rId1"/>
-    <sheet name="BE" sheetId="2" r:id="rId2"/>
-    <sheet name="BG" sheetId="3" r:id="rId3"/>
-    <sheet name="HR" sheetId="4" r:id="rId4"/>
-    <sheet name="CZ" sheetId="5" r:id="rId5"/>
-    <sheet name="DK" sheetId="6" r:id="rId6"/>
-    <sheet name="EE" sheetId="7" r:id="rId7"/>
-    <sheet name="FI" sheetId="8" r:id="rId8"/>
-    <sheet name="FR" sheetId="9" r:id="rId9"/>
-    <sheet name="DE" sheetId="10" r:id="rId10"/>
-    <sheet name="EL" sheetId="11" r:id="rId11"/>
-    <sheet name="IE" sheetId="12" r:id="rId12"/>
-    <sheet name="HU" sheetId="13" r:id="rId13"/>
-    <sheet name="IT" sheetId="14" r:id="rId14"/>
-    <sheet name="LV" sheetId="15" r:id="rId15"/>
-    <sheet name="LT" sheetId="16" r:id="rId16"/>
-    <sheet name="LU" sheetId="17" r:id="rId17"/>
-    <sheet name="NL" sheetId="18" r:id="rId18"/>
-    <sheet name="NO" sheetId="19" r:id="rId19"/>
-    <sheet name="PL" sheetId="20" r:id="rId20"/>
-    <sheet name="PT" sheetId="21" r:id="rId21"/>
-    <sheet name="RO" sheetId="22" r:id="rId22"/>
-    <sheet name="SK" sheetId="23" r:id="rId23"/>
-    <sheet name="SI" sheetId="24" r:id="rId24"/>
-    <sheet name="ES" sheetId="25" r:id="rId25"/>
-    <sheet name="CH" sheetId="26" r:id="rId26"/>
-    <sheet name="SE" sheetId="27" r:id="rId27"/>
-    <sheet name="UK" sheetId="28" r:id="rId28"/>
-    <sheet name="ALL" sheetId="29" r:id="rId29"/>
+    <sheet name="ALL" sheetId="1" r:id="rId1"/>
+    <sheet name="AT" sheetId="2" r:id="rId2"/>
+    <sheet name="BE" sheetId="3" r:id="rId3"/>
+    <sheet name="BG" sheetId="4" r:id="rId4"/>
+    <sheet name="CH" sheetId="5" r:id="rId5"/>
+    <sheet name="CZ" sheetId="6" r:id="rId6"/>
+    <sheet name="DE" sheetId="7" r:id="rId7"/>
+    <sheet name="DK" sheetId="8" r:id="rId8"/>
+    <sheet name="EE" sheetId="9" r:id="rId9"/>
+    <sheet name="EL" sheetId="10" r:id="rId10"/>
+    <sheet name="ES" sheetId="11" r:id="rId11"/>
+    <sheet name="FI" sheetId="12" r:id="rId12"/>
+    <sheet name="FR" sheetId="13" r:id="rId13"/>
+    <sheet name="HR" sheetId="14" r:id="rId14"/>
+    <sheet name="HU" sheetId="15" r:id="rId15"/>
+    <sheet name="IE" sheetId="16" r:id="rId16"/>
+    <sheet name="IT" sheetId="17" r:id="rId17"/>
+    <sheet name="LT" sheetId="18" r:id="rId18"/>
+    <sheet name="LU" sheetId="19" r:id="rId19"/>
+    <sheet name="LV" sheetId="20" r:id="rId20"/>
+    <sheet name="NL" sheetId="21" r:id="rId21"/>
+    <sheet name="NO" sheetId="22" r:id="rId22"/>
+    <sheet name="PL" sheetId="23" r:id="rId23"/>
+    <sheet name="PT" sheetId="24" r:id="rId24"/>
+    <sheet name="RO" sheetId="25" r:id="rId25"/>
+    <sheet name="SE" sheetId="26" r:id="rId26"/>
+    <sheet name="SI" sheetId="27" r:id="rId27"/>
+    <sheet name="SK" sheetId="28" r:id="rId28"/>
+    <sheet name="UK" sheetId="29" r:id="rId29"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -457,19 +457,19 @@
         <v>2000</v>
       </c>
       <c r="C2">
-        <v>11613</v>
+        <v>155303.3</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>198.1</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>62.95</v>
       </c>
       <c r="G2">
-        <v>50</v>
+        <v>12250.57</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -480,19 +480,19 @@
         <v>2005</v>
       </c>
       <c r="C3">
-        <v>186.0400000000009</v>
+        <v>3891.820000000007</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>16.02</v>
+        <v>2105.09</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>407.6</v>
       </c>
       <c r="G3">
-        <v>775.22</v>
+        <v>26316.14</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -503,19 +503,19 @@
         <v>2010</v>
       </c>
       <c r="C4">
-        <v>1095.809999999999</v>
+        <v>4973.239999999991</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>738.72</v>
       </c>
       <c r="E4">
-        <v>67.8</v>
+        <v>27706.06999999999</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1118.6</v>
       </c>
       <c r="G4">
-        <v>190.61</v>
+        <v>39165.92999999999</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -526,19 +526,19 @@
         <v>2015</v>
       </c>
       <c r="C5">
-        <v>754.8099999999995</v>
+        <v>5818.410000000033</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1573.41</v>
       </c>
       <c r="E5">
-        <v>848.28</v>
+        <v>56635.87000000001</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>4313.400000000001</v>
       </c>
       <c r="G5">
-        <v>1472.9</v>
+        <v>44304.63999999998</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -549,19 +549,19 @@
         <v>2019</v>
       </c>
       <c r="C6">
-        <v>947.4500000000007</v>
+        <v>6085.600000000006</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>9.040000000000418</v>
       </c>
       <c r="E6">
-        <v>765.0000000000002</v>
+        <v>33724.74000000001</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>6157.249999999999</v>
       </c>
       <c r="G6">
-        <v>735.3899999999999</v>
+        <v>35871.71000000005</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -572,19 +572,19 @@
         <v>2020</v>
       </c>
       <c r="C7">
-        <v>550</v>
+        <v>695.4699999999721</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>517.9999999999998</v>
+        <v>18956.66999999997</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>2477.4</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>8227.880000000005</v>
       </c>
     </row>
   </sheetData>
@@ -631,19 +631,19 @@
         <v>2000</v>
       </c>
       <c r="C2">
-        <v>4831</v>
+        <v>3072</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>114</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>6095</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -654,19 +654,19 @@
         <v>2005</v>
       </c>
       <c r="C3">
-        <v>379</v>
+        <v>34</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>1942</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>12153</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -677,19 +677,19 @@
         <v>2010</v>
       </c>
       <c r="C4">
-        <v>197</v>
+        <v>109</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>15948</v>
+        <v>201</v>
       </c>
       <c r="F4">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>8575</v>
+        <v>807</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -700,19 +700,19 @@
         <v>2015</v>
       </c>
       <c r="C5">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>21218</v>
+        <v>2402</v>
       </c>
       <c r="F5">
-        <v>3203</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>14474</v>
+        <v>793</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -723,19 +723,19 @@
         <v>2019</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>9823</v>
+        <v>229.79</v>
       </c>
       <c r="F6">
-        <v>4245</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>11896</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -752,13 +752,13 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>4736</v>
+        <v>413.21</v>
       </c>
       <c r="F7">
-        <v>219</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>1244</v>
+        <v>524</v>
       </c>
     </row>
   </sheetData>
@@ -805,19 +805,19 @@
         <v>2000</v>
       </c>
       <c r="C2">
-        <v>3072</v>
+        <v>15542</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>226</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -828,19 +828,19 @@
         <v>2005</v>
       </c>
       <c r="C3">
-        <v>34</v>
+        <v>254</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>265</v>
+        <v>7712</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -851,19 +851,19 @@
         <v>2010</v>
       </c>
       <c r="C4">
-        <v>109</v>
+        <v>290</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>732</v>
       </c>
       <c r="E4">
-        <v>201</v>
+        <v>3821</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>807</v>
+        <v>10775</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -874,19 +874,19 @@
         <v>2015</v>
       </c>
       <c r="C5">
-        <v>177</v>
+        <v>687</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1572.06</v>
       </c>
       <c r="E5">
-        <v>2402</v>
+        <v>831</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G5">
-        <v>793</v>
+        <v>2245</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -897,19 +897,19 @@
         <v>2019</v>
       </c>
       <c r="C6">
-        <v>20</v>
+        <v>19.66999999999825</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>229.79</v>
+        <v>4268.51</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>1498</v>
+        <v>2640.150000000001</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -926,13 +926,13 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>413.21</v>
+        <v>2812.5</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>524</v>
+        <v>1505.689999999999</v>
       </c>
     </row>
   </sheetData>
@@ -979,19 +979,19 @@
         <v>2000</v>
       </c>
       <c r="C2">
-        <v>236</v>
+        <v>2882</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>116.5</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1002,19 +1002,19 @@
         <v>2005</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>153</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F3">
-        <v>25.2</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>351.6</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1025,19 +1025,19 @@
         <v>2010</v>
       </c>
       <c r="C4">
+        <v>120</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
         <v>3</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0.6899999999999999</v>
-      </c>
       <c r="F4">
-        <v>0</v>
+        <v>26.3</v>
       </c>
       <c r="G4">
-        <v>897.1</v>
+        <v>88.69999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1048,19 +1048,19 @@
         <v>2015</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>94</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>1.66</v>
+        <v>10</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>5.699999999999999</v>
       </c>
       <c r="G5">
-        <v>1060.75</v>
+        <v>802.3</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1071,19 +1071,19 @@
         <v>2019</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>28.76</v>
+        <v>205</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="G6">
-        <v>1708.8</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1094,19 +1094,19 @@
         <v>2020</v>
       </c>
       <c r="C7">
-        <v>0.2299999999999898</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>9.079999999999998</v>
+        <v>169</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>139.9099999999999</v>
+        <v>190.1999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -1153,19 +1153,19 @@
         <v>2000</v>
       </c>
       <c r="C2">
-        <v>48</v>
+        <v>23297</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1176,19 +1176,19 @@
         <v>2005</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>17</v>
+        <v>652</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1199,19 +1199,19 @@
         <v>2010</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>288</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>1031</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>276</v>
+        <v>5222</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1222,19 +1222,19 @@
         <v>2015</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>207.1700000000019</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>170</v>
+        <v>6093.52</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>36</v>
+        <v>4386.18</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1245,19 +1245,19 @@
         <v>2019</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>316.7099999999991</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E6">
-        <v>1228</v>
+        <v>3657.93</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>6126.669999999998</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1268,19 +1268,19 @@
         <v>2020</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>28.19999999999709</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>553</v>
+        <v>929</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>955</v>
       </c>
     </row>
   </sheetData>
@@ -1327,19 +1327,19 @@
         <v>2000</v>
       </c>
       <c r="C2">
-        <v>16390</v>
+        <v>2067</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>363</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1350,19 +1350,19 @@
         <v>2005</v>
       </c>
       <c r="C3">
-        <v>646</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>1272</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1373,19 +1373,19 @@
         <v>2010</v>
       </c>
       <c r="C4">
-        <v>527</v>
+        <v>64</v>
       </c>
       <c r="D4">
-        <v>4.72</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>3558</v>
+        <v>0.3</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>4159</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1396,19 +1396,19 @@
         <v>2015</v>
       </c>
       <c r="C5">
-        <v>675</v>
+        <v>66.09999999999991</v>
       </c>
       <c r="D5">
-        <v>1.350000000000001</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>15309</v>
+        <v>47.5</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>3343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1419,19 +1419,19 @@
         <v>2019</v>
       </c>
       <c r="C6">
-        <v>362.7099999999991</v>
+        <v>4.599999999999909</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>1964.279999999999</v>
+        <v>37</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>1542.459999999999</v>
+        <v>228.3</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1448,13 +1448,13 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>729</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>160</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1501,7 +1501,7 @@
         <v>2000</v>
       </c>
       <c r="C2">
-        <v>1513</v>
+        <v>48</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1513,7 +1513,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1524,7 +1524,7 @@
         <v>2005</v>
       </c>
       <c r="C3">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1536,7 +1536,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1547,19 +1547,19 @@
         <v>2010</v>
       </c>
       <c r="C4">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>4</v>
+        <v>276</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1570,19 +1570,19 @@
         <v>2015</v>
       </c>
       <c r="C5">
-        <v>11.69000000000005</v>
+        <v>4</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0.2</v>
+        <v>170</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>38.17</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1593,19 +1593,19 @@
         <v>2019</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>3.1</v>
+        <v>1228</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>9.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1622,7 +1622,7 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>3.9</v>
+        <v>553</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1675,7 +1675,7 @@
         <v>2000</v>
       </c>
       <c r="C2">
-        <v>103</v>
+        <v>236</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1687,7 +1687,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>116.5</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1698,7 +1698,7 @@
         <v>2005</v>
       </c>
       <c r="C3">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1707,10 +1707,10 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>25.2</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>351.6</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1721,19 +1721,19 @@
         <v>2010</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0.1</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>132</v>
+        <v>897.1</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1744,19 +1744,19 @@
         <v>2015</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>68.90000000000001</v>
+        <v>1.66</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>303</v>
+        <v>1060.75</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1773,13 +1773,13 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>13</v>
+        <v>28.76</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>97</v>
+        <v>1708.8</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1790,19 +1790,19 @@
         <v>2020</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>0.2299999999999898</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>66</v>
+        <v>9.079999999999998</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>6</v>
+        <v>139.9099999999999</v>
       </c>
     </row>
   </sheetData>
@@ -1849,19 +1849,19 @@
         <v>2000</v>
       </c>
       <c r="C2">
-        <v>33.3</v>
+        <v>16390</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>14</v>
+        <v>363</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1872,19 +1872,19 @@
         <v>2005</v>
       </c>
       <c r="C3">
-        <v>0.7800000000000011</v>
+        <v>646</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>23.58</v>
+        <v>15</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>20.9</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1895,19 +1895,19 @@
         <v>2010</v>
       </c>
       <c r="C4">
-        <v>0.230000000000004</v>
+        <v>527</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>4.72</v>
       </c>
       <c r="E4">
-        <v>5.870000000000001</v>
+        <v>3558</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>8.829999999999998</v>
+        <v>4159</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1918,19 +1918,19 @@
         <v>2015</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>675</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1.350000000000001</v>
       </c>
       <c r="E5">
-        <v>86.81999999999999</v>
+        <v>15309</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>20.06</v>
+        <v>3343</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1941,19 +1941,19 @@
         <v>2019</v>
       </c>
       <c r="C6">
-        <v>0.1999999999999957</v>
+        <v>362.7099999999991</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>43.47000000000001</v>
+        <v>1964.279999999999</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>72</v>
+        <v>1542.459999999999</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1970,13 +1970,13 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>35</v>
+        <v>729</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>30.21000000000001</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -2023,19 +2023,19 @@
         <v>2000</v>
       </c>
       <c r="C2">
-        <v>37</v>
+        <v>103</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>447</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2046,19 +2046,19 @@
         <v>2005</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>777</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2075,13 +2075,13 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>39</v>
+        <v>0.1</v>
       </c>
       <c r="F4">
-        <v>228</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>785</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2092,19 +2092,19 @@
         <v>2015</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>1436</v>
+        <v>68.90000000000001</v>
       </c>
       <c r="F5">
-        <v>129</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>1025</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2121,13 +2121,13 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>5651</v>
+        <v>13</v>
       </c>
       <c r="F6">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>493</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2144,13 +2144,13 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>3036</v>
+        <v>66</v>
       </c>
       <c r="F7">
-        <v>1543</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>573</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -2197,19 +2197,19 @@
         <v>2000</v>
       </c>
       <c r="C2">
-        <v>28126</v>
+        <v>33.3</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2220,19 +2220,19 @@
         <v>2005</v>
       </c>
       <c r="C3">
-        <v>423</v>
+        <v>0.7800000000000011</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>23.58</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>252</v>
+        <v>20.9</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2243,19 +2243,19 @@
         <v>2010</v>
       </c>
       <c r="C4">
-        <v>1144</v>
+        <v>0.230000000000004</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>2.1</v>
+        <v>5.870000000000001</v>
       </c>
       <c r="F4">
-        <v>2.3</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>157.7</v>
+        <v>8.829999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2266,19 +2266,19 @@
         <v>2015</v>
       </c>
       <c r="C5">
-        <v>1679</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>5.9</v>
+        <v>86.81999999999999</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>442.0000000000001</v>
+        <v>20.06</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2289,19 +2289,19 @@
         <v>2019</v>
       </c>
       <c r="C6">
-        <v>1425</v>
+        <v>0.1999999999999957</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>105</v>
+        <v>43.47000000000001</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>2047</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2312,19 +2312,19 @@
         <v>2020</v>
       </c>
       <c r="C7">
-        <v>206</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>31.69999999999999</v>
+        <v>35</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>1063</v>
+        <v>30.21000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -2371,19 +2371,19 @@
         <v>2000</v>
       </c>
       <c r="C2">
-        <v>103</v>
+        <v>11613</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>14</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2394,19 +2394,19 @@
         <v>2005</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>186.0400000000009</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>16.02</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>153</v>
+        <v>775.22</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2417,19 +2417,19 @@
         <v>2010</v>
       </c>
       <c r="C4">
-        <v>13</v>
+        <v>1095.809999999999</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1004.6</v>
+        <v>67.8</v>
       </c>
       <c r="F4">
-        <v>196.5</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>548.5</v>
+        <v>190.61</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2440,19 +2440,19 @@
         <v>2015</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>754.8099999999995</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>2125</v>
+        <v>848.28</v>
       </c>
       <c r="F5">
-        <v>515.5</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>748.5</v>
+        <v>1472.9</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2463,19 +2463,19 @@
         <v>2019</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>947.4500000000007</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>1505</v>
+        <v>765.0000000000002</v>
       </c>
       <c r="F6">
-        <v>843.5</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>843.9000000000001</v>
+        <v>735.3899999999999</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2486,19 +2486,19 @@
         <v>2020</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>550</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>1009.799999999999</v>
+        <v>517.9999999999998</v>
       </c>
       <c r="F7">
-        <v>698.4000000000001</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>129.9200000000001</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2545,7 +2545,7 @@
         <v>2000</v>
       </c>
       <c r="C2">
-        <v>817</v>
+        <v>1513</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -2557,7 +2557,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2568,7 +2568,7 @@
         <v>2005</v>
       </c>
       <c r="C3">
-        <v>98</v>
+        <v>23</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -2580,7 +2580,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>117</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2591,7 +2591,7 @@
         <v>2010</v>
       </c>
       <c r="C4">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -2603,7 +2603,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>987</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2614,19 +2614,19 @@
         <v>2015</v>
       </c>
       <c r="C5">
-        <v>28</v>
+        <v>11.69000000000005</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>107.78</v>
+        <v>0.2</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>3778</v>
+        <v>38.17</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2637,19 +2637,19 @@
         <v>2019</v>
       </c>
       <c r="C6">
-        <v>9.509999999999991</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>1431.48</v>
+        <v>3.1</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>950.8199999999997</v>
+        <v>9.75</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2660,19 +2660,19 @@
         <v>2020</v>
       </c>
       <c r="C7">
-        <v>2.950000000000045</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>2396.48</v>
+        <v>3.9</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>429.8699999999999</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2719,19 +2719,19 @@
         <v>2000</v>
       </c>
       <c r="C2">
-        <v>4535</v>
+        <v>37</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>83</v>
+        <v>447</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2742,19 +2742,19 @@
         <v>2005</v>
       </c>
       <c r="C3">
-        <v>482</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>981</v>
+        <v>777</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2765,19 +2765,19 @@
         <v>2010</v>
       </c>
       <c r="C4">
-        <v>89</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>132</v>
+        <v>39</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>228</v>
       </c>
       <c r="G4">
-        <v>2732</v>
+        <v>785</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2788,19 +2788,19 @@
         <v>2015</v>
       </c>
       <c r="C5">
-        <v>1062</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>313</v>
+        <v>1436</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>129</v>
       </c>
       <c r="G5">
-        <v>1138.84</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2811,19 +2811,19 @@
         <v>2019</v>
       </c>
       <c r="C6">
-        <v>1093.99</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>454.4400000000001</v>
+        <v>5651</v>
       </c>
       <c r="F6">
-        <v>6</v>
+        <v>600</v>
       </c>
       <c r="G6">
-        <v>279.9099999999999</v>
+        <v>493</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2840,13 +2840,13 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>124</v>
+        <v>3036</v>
       </c>
       <c r="F7">
-        <v>17</v>
+        <v>1543</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>573</v>
       </c>
     </row>
   </sheetData>
@@ -2893,19 +2893,19 @@
         <v>2000</v>
       </c>
       <c r="C2">
-        <v>6120</v>
+        <v>28126</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2916,19 +2916,19 @@
         <v>2005</v>
       </c>
       <c r="C3">
-        <v>169</v>
+        <v>423</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2939,19 +2939,19 @@
         <v>2010</v>
       </c>
       <c r="C4">
-        <v>93</v>
+        <v>1144</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0.1</v>
+        <v>2.1</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>2.3</v>
       </c>
       <c r="G4">
-        <v>388</v>
+        <v>157.7</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2962,19 +2962,19 @@
         <v>2015</v>
       </c>
       <c r="C5">
-        <v>256</v>
+        <v>1679</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>1325.9</v>
+        <v>5.9</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>2741</v>
+        <v>442.0000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2985,19 +2985,19 @@
         <v>2019</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1425</v>
       </c>
       <c r="D6">
-        <v>0.09</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>71.71000000000004</v>
+        <v>105</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -3008,19 +3008,19 @@
         <v>2020</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>206</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>31.69999999999999</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>1063</v>
       </c>
     </row>
   </sheetData>
@@ -3067,7 +3067,7 @@
         <v>2000</v>
       </c>
       <c r="C2">
-        <v>1685</v>
+        <v>817</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -3079,7 +3079,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -3090,7 +3090,7 @@
         <v>2005</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -3102,7 +3102,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>5</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -3113,19 +3113,19 @@
         <v>2010</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>987</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -3136,19 +3136,19 @@
         <v>2015</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>514</v>
+        <v>107.78</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>3778</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -3159,19 +3159,19 @@
         <v>2019</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>9.509999999999991</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>57</v>
+        <v>1431.48</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>950.8199999999997</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -3182,19 +3182,19 @@
         <v>2020</v>
       </c>
       <c r="C7">
-        <v>0.7000000000000455</v>
+        <v>2.950000000000045</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>2.899999999999977</v>
+        <v>2396.48</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>429.8699999999999</v>
       </c>
     </row>
   </sheetData>
@@ -3241,7 +3241,7 @@
         <v>2000</v>
       </c>
       <c r="C2">
-        <v>843</v>
+        <v>4535</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -3253,7 +3253,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -3264,19 +3264,19 @@
         <v>2005</v>
       </c>
       <c r="C3">
-        <v>136</v>
+        <v>482</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>981</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -3287,19 +3287,19 @@
         <v>2010</v>
       </c>
       <c r="C4">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>11</v>
+        <v>132</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>2732</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -3310,19 +3310,19 @@
         <v>2015</v>
       </c>
       <c r="C5">
-        <v>41</v>
+        <v>1062</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>226</v>
+        <v>313</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>1138.84</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -3333,19 +3333,19 @@
         <v>2019</v>
       </c>
       <c r="C6">
-        <v>55.72000000000003</v>
+        <v>1093.99</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>25.81</v>
+        <v>454.4400000000001</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G6">
-        <v>0.3499999999999996</v>
+        <v>279.9099999999999</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -3362,10 +3362,10 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -3415,19 +3415,19 @@
         <v>2000</v>
       </c>
       <c r="C2">
-        <v>15542</v>
+        <v>6120</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>2206</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -3438,19 +3438,19 @@
         <v>2005</v>
       </c>
       <c r="C3">
-        <v>254</v>
+        <v>169</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>7712</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -3461,19 +3461,19 @@
         <v>2010</v>
       </c>
       <c r="C4">
-        <v>290</v>
+        <v>93</v>
       </c>
       <c r="D4">
-        <v>732</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>3821</v>
+        <v>0.1</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>10775</v>
+        <v>388</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -3484,19 +3484,19 @@
         <v>2015</v>
       </c>
       <c r="C5">
-        <v>687</v>
+        <v>256</v>
       </c>
       <c r="D5">
-        <v>1572.06</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>831</v>
+        <v>1325.9</v>
       </c>
       <c r="F5">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>2245</v>
+        <v>2741</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -3507,19 +3507,19 @@
         <v>2019</v>
       </c>
       <c r="C6">
-        <v>19.66999999999825</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="E6">
-        <v>4268.51</v>
+        <v>71.71000000000004</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>2640.150000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -3536,13 +3536,13 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>2812.5</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>1505.689999999999</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3589,19 +3589,19 @@
         <v>2000</v>
       </c>
       <c r="C2">
-        <v>12924</v>
+        <v>16506</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G2">
-        <v>3</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -3612,19 +3612,19 @@
         <v>2005</v>
       </c>
       <c r="C3">
-        <v>116</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G3">
-        <v>9</v>
+        <v>304</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -3635,19 +3635,19 @@
         <v>2010</v>
       </c>
       <c r="C4">
-        <v>227</v>
+        <v>322</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>97</v>
+        <v>7</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>141</v>
       </c>
       <c r="G4">
-        <v>30</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -3658,19 +3658,19 @@
         <v>2015</v>
       </c>
       <c r="C5">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>1269</v>
+        <v>93</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G5">
-        <v>18</v>
+        <v>3752</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -3681,19 +3681,19 @@
         <v>2019</v>
       </c>
       <c r="C6">
-        <v>1666</v>
+        <v>232</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>1104</v>
+        <v>610</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>15</v>
+        <v>2872</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -3704,19 +3704,19 @@
         <v>2020</v>
       </c>
       <c r="C7">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>445.25</v>
+        <v>703.1500000000001</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>12</v>
+        <v>1007</v>
       </c>
     </row>
   </sheetData>
@@ -3763,19 +3763,19 @@
         <v>2000</v>
       </c>
       <c r="C2">
-        <v>16506</v>
+        <v>843</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>196</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -3786,19 +3786,19 @@
         <v>2005</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>136</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>304</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -3809,19 +3809,19 @@
         <v>2010</v>
       </c>
       <c r="C4">
-        <v>322</v>
+        <v>95</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F4">
-        <v>141</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>1354</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -3832,19 +3832,19 @@
         <v>2015</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>93</v>
+        <v>226</v>
       </c>
       <c r="F5">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>3752</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -3855,19 +3855,19 @@
         <v>2019</v>
       </c>
       <c r="C6">
-        <v>232</v>
+        <v>55.72000000000003</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>610</v>
+        <v>25.81</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>2872</v>
+        <v>0.3499999999999996</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -3878,19 +3878,19 @@
         <v>2020</v>
       </c>
       <c r="C7">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>703.1500000000001</v>
+        <v>3</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>1007</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3899,6 +3899,180 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>2020</v>
+      </c>
+      <c r="B2">
+        <v>2000</v>
+      </c>
+      <c r="C2">
+        <v>1685</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>2020</v>
+      </c>
+      <c r="B3">
+        <v>2005</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>2020</v>
+      </c>
+      <c r="B4">
+        <v>2010</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>19</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>2020</v>
+      </c>
+      <c r="B5">
+        <v>2015</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>514</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>2020</v>
+      </c>
+      <c r="B6">
+        <v>2019</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>57</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>2020</v>
+      </c>
+      <c r="B7">
+        <v>2020</v>
+      </c>
+      <c r="C7">
+        <v>0.7000000000000455</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>2.899999999999977</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B1"/>
   <sheetViews>
@@ -3912,180 +4086,6 @@
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2">
-        <v>2020</v>
-      </c>
-      <c r="B2">
-        <v>2000</v>
-      </c>
-      <c r="C2">
-        <v>155303.3</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>198.1</v>
-      </c>
-      <c r="F2">
-        <v>62.95</v>
-      </c>
-      <c r="G2">
-        <v>12250.57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3">
-        <v>2020</v>
-      </c>
-      <c r="B3">
-        <v>2005</v>
-      </c>
-      <c r="C3">
-        <v>3891.820000000007</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>2105.09</v>
-      </c>
-      <c r="F3">
-        <v>407.6</v>
-      </c>
-      <c r="G3">
-        <v>26316.14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4">
-        <v>2020</v>
-      </c>
-      <c r="B4">
-        <v>2010</v>
-      </c>
-      <c r="C4">
-        <v>4973.239999999991</v>
-      </c>
-      <c r="D4">
-        <v>738.72</v>
-      </c>
-      <c r="E4">
-        <v>27706.06999999999</v>
-      </c>
-      <c r="F4">
-        <v>1118.6</v>
-      </c>
-      <c r="G4">
-        <v>39165.92999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5">
-        <v>2020</v>
-      </c>
-      <c r="B5">
-        <v>2015</v>
-      </c>
-      <c r="C5">
-        <v>5818.410000000033</v>
-      </c>
-      <c r="D5">
-        <v>1573.41</v>
-      </c>
-      <c r="E5">
-        <v>56635.87000000001</v>
-      </c>
-      <c r="F5">
-        <v>4313.400000000001</v>
-      </c>
-      <c r="G5">
-        <v>44304.63999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6">
-        <v>2020</v>
-      </c>
-      <c r="B6">
-        <v>2019</v>
-      </c>
-      <c r="C6">
-        <v>6085.600000000006</v>
-      </c>
-      <c r="D6">
-        <v>9.040000000000418</v>
-      </c>
-      <c r="E6">
-        <v>33724.74000000001</v>
-      </c>
-      <c r="F6">
-        <v>6157.249999999999</v>
-      </c>
-      <c r="G6">
-        <v>35871.71000000005</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7">
-        <v>2020</v>
-      </c>
-      <c r="B7">
-        <v>2020</v>
-      </c>
-      <c r="C7">
-        <v>695.4699999999721</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>18956.66999999997</v>
-      </c>
-      <c r="F7">
-        <v>2477.4</v>
-      </c>
-      <c r="G7">
-        <v>8227.880000000005</v>
       </c>
     </row>
   </sheetData>
@@ -4132,7 +4132,7 @@
         <v>2000</v>
       </c>
       <c r="C2">
-        <v>1016</v>
+        <v>103</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -4144,7 +4144,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -4155,19 +4155,19 @@
         <v>2005</v>
       </c>
       <c r="C3">
-        <v>968</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>8</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -4178,19 +4178,19 @@
         <v>2010</v>
       </c>
       <c r="C4">
-        <v>200</v>
+        <v>13</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>25</v>
+        <v>1004.6</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>196.5</v>
       </c>
       <c r="G4">
-        <v>480</v>
+        <v>548.5</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -4201,19 +4201,19 @@
         <v>2015</v>
       </c>
       <c r="C5">
-        <v>171</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>1004</v>
+        <v>2125</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>515.5</v>
       </c>
       <c r="G5">
-        <v>211</v>
+        <v>748.5</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -4224,19 +4224,19 @@
         <v>2019</v>
       </c>
       <c r="C6">
-        <v>159.3499999999999</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>18.95000000000005</v>
+        <v>1505</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>843.5</v>
       </c>
       <c r="G6">
-        <v>4.120000000000005</v>
+        <v>843.9000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -4247,19 +4247,19 @@
         <v>2020</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>25</v>
+        <v>1009.799999999999</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>698.4000000000001</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>129.9200000000001</v>
       </c>
     </row>
   </sheetData>
@@ -4306,7 +4306,7 @@
         <v>2000</v>
       </c>
       <c r="C2">
-        <v>2067</v>
+        <v>1016</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -4329,7 +4329,7 @@
         <v>2005</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>968</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -4341,7 +4341,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -4352,19 +4352,19 @@
         <v>2010</v>
       </c>
       <c r="C4">
-        <v>64</v>
+        <v>200</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0.3</v>
+        <v>25</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>73</v>
+        <v>480</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -4375,19 +4375,19 @@
         <v>2015</v>
       </c>
       <c r="C5">
-        <v>66.09999999999991</v>
+        <v>171</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>47.5</v>
+        <v>1004</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>339</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -4398,19 +4398,19 @@
         <v>2019</v>
       </c>
       <c r="C6">
-        <v>4.599999999999909</v>
+        <v>159.3499999999999</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>37</v>
+        <v>18.95000000000005</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>228.3</v>
+        <v>4.120000000000005</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -4427,13 +4427,13 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>142</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4480,19 +4480,19 @@
         <v>2000</v>
       </c>
       <c r="C2">
-        <v>952</v>
+        <v>12924</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0.1</v>
+        <v>16</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -4503,19 +4503,19 @@
         <v>2005</v>
       </c>
       <c r="C3">
-        <v>68</v>
+        <v>116</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0.49</v>
+        <v>12</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -4526,19 +4526,19 @@
         <v>2010</v>
       </c>
       <c r="C4">
-        <v>29</v>
+        <v>227</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1726.41</v>
+        <v>97</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>191</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -4549,19 +4549,19 @@
         <v>2015</v>
       </c>
       <c r="C5">
-        <v>39</v>
+        <v>79</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>347.9000000000001</v>
+        <v>1269</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>68</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -4572,19 +4572,19 @@
         <v>2019</v>
       </c>
       <c r="C6">
-        <v>5.710000000000036</v>
+        <v>1666</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>11.51999999999998</v>
+        <v>1104</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>58.41000000000003</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -4595,19 +4595,19 @@
         <v>2020</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>445.25</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -4654,19 +4654,19 @@
         <v>2000</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>952</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="F2">
-        <v>49.95</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>2340.07</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -4677,19 +4677,19 @@
         <v>2005</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>68</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>0.49</v>
       </c>
       <c r="F3">
-        <v>373.4</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>364.4199999999996</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -4700,19 +4700,19 @@
         <v>2010</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>4</v>
+        <v>1726.41</v>
       </c>
       <c r="F4">
-        <v>444.5</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>229.4900000000002</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -4723,19 +4723,19 @@
         <v>2015</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>775.11</v>
+        <v>347.9000000000001</v>
       </c>
       <c r="F5">
-        <v>403.1999999999999</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>871.9400000000001</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -4746,19 +4746,19 @@
         <v>2019</v>
       </c>
       <c r="C6">
-        <v>0.3799999999999999</v>
+        <v>5.710000000000036</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>297.89</v>
+        <v>11.51999999999998</v>
       </c>
       <c r="F6">
-        <v>429.75</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>596.1599999999999</v>
+        <v>58.41000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -4775,13 +4775,13 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>220</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>132.0799999999999</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4828,19 +4828,19 @@
         <v>2000</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>4831</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>6095</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -4851,19 +4851,19 @@
         <v>2005</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>379</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1942</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>31</v>
+        <v>12153</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -4874,19 +4874,19 @@
         <v>2010</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>197</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>0.1</v>
+        <v>15948</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G4">
-        <v>77</v>
+        <v>8575</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -4897,19 +4897,19 @@
         <v>2015</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>182</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>6.4</v>
+        <v>21218</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>3203</v>
       </c>
       <c r="G5">
-        <v>192</v>
+        <v>14474</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -4926,13 +4926,13 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>114.1</v>
+        <v>9823</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>4245</v>
       </c>
       <c r="G6">
-        <v>16</v>
+        <v>11896</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -4943,19 +4943,19 @@
         <v>2020</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>9.700000000000017</v>
+        <v>4736</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>219</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>1244</v>
       </c>
     </row>
   </sheetData>
@@ -5002,19 +5002,19 @@
         <v>2000</v>
       </c>
       <c r="C2">
-        <v>2882</v>
+        <v>10</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>49.95</v>
       </c>
       <c r="G2">
-        <v>38</v>
+        <v>2340.07</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -5025,7 +5025,7 @@
         <v>2005</v>
       </c>
       <c r="C3">
-        <v>153</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -5034,10 +5034,10 @@
         <v>2</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>373.4</v>
       </c>
       <c r="G3">
-        <v>44</v>
+        <v>364.4199999999996</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -5048,19 +5048,19 @@
         <v>2010</v>
       </c>
       <c r="C4">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F4">
-        <v>26.3</v>
+        <v>444.5</v>
       </c>
       <c r="G4">
-        <v>88.69999999999999</v>
+        <v>229.4900000000002</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -5071,19 +5071,19 @@
         <v>2015</v>
       </c>
       <c r="C5">
-        <v>94</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>10</v>
+        <v>775.11</v>
       </c>
       <c r="F5">
-        <v>5.699999999999999</v>
+        <v>403.1999999999999</v>
       </c>
       <c r="G5">
-        <v>802.3</v>
+        <v>871.9400000000001</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -5094,19 +5094,19 @@
         <v>2019</v>
       </c>
       <c r="C6">
-        <v>24</v>
+        <v>0.3799999999999999</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>205</v>
+        <v>297.89</v>
       </c>
       <c r="F6">
-        <v>41</v>
+        <v>429.75</v>
       </c>
       <c r="G6">
-        <v>1238</v>
+        <v>596.1599999999999</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -5123,13 +5123,13 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>169</v>
+        <v>220</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>190.1999999999998</v>
+        <v>132.0799999999999</v>
       </c>
     </row>
   </sheetData>
@@ -5176,19 +5176,19 @@
         <v>2000</v>
       </c>
       <c r="C2">
-        <v>23297</v>
+        <v>2</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>38</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -5199,19 +5199,19 @@
         <v>2005</v>
       </c>
       <c r="C3">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>652</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -5222,19 +5222,19 @@
         <v>2010</v>
       </c>
       <c r="C4">
-        <v>288</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1031</v>
+        <v>0.1</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>5222</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -5245,19 +5245,19 @@
         <v>2015</v>
       </c>
       <c r="C5">
-        <v>207.1700000000019</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>6093.52</v>
+        <v>6.4</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>4386.18</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -5268,19 +5268,19 @@
         <v>2019</v>
       </c>
       <c r="C6">
-        <v>316.7099999999991</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>3657.93</v>
+        <v>114.1</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>6126.669999999998</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -5291,19 +5291,19 @@
         <v>2020</v>
       </c>
       <c r="C7">
-        <v>28.19999999999709</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>929</v>
+        <v>9.700000000000017</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>955</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>